<commit_message>
Schematic Completed, All components except for lightning port added to libraries
</commit_message>
<xml_diff>
--- a/Documentation/Component Purchasing.xlsx
+++ b/Documentation/Component Purchasing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC104887E99C63F05ADE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{41B5622B-A326-4D5C-99A1-4D3C30A4E378}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="3285" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-[$$-1009]* #,##0.00_-;\-[$$-1009]* #,##0.00_-;_-[$$-1009]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -149,14 +149,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
         <v>6.45</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H13" si="0">F3*G3</f>
+        <f t="shared" ref="H3:H4" si="0">F3*G3</f>
         <v>32.25</v>
       </c>
     </row>

</xml_diff>